<commit_message>
fix out of stock item in bom
</commit_message>
<xml_diff>
--- a/bom/BOM_BAUDIO_v1.1.xlsx
+++ b/bom/BOM_BAUDIO_v1.1.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,22 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/simonb/src/baudio/bom/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{BA86C868-7596-824F-A6E3-0E47A3DBC1DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB110293-E25F-DA47-B5F5-CD75CDA50A19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="960" windowWidth="27640" windowHeight="16940"/>
+    <workbookView xWindow="2780" yWindow="960" windowWidth="27640" windowHeight="16940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM_Bcard2024_2024-03-20" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'BOM_Bcard2024_2024-03-20'!$A$1:$I$37</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'BOM_Bcard2024_2024-03-20'!$A$1:$I$36</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="161">
   <si>
     <t>ID</t>
   </si>
@@ -319,15 +319,9 @@
     <t>HDR-M-2.54_1x3</t>
   </si>
   <si>
-    <t>FSEL,AMP,DAC,LINE-IN</t>
-  </si>
-  <si>
     <t>HDR-M-2.54_1X3</t>
   </si>
   <si>
-    <t>C180248</t>
-  </si>
-  <si>
     <t>Black headphone jack</t>
   </si>
   <si>
@@ -361,9 +355,6 @@
     <t>C614831</t>
   </si>
   <si>
-    <t>OUT2</t>
-  </si>
-  <si>
     <t>CASE-A_3216</t>
   </si>
   <si>
@@ -509,12 +500,18 @@
   </si>
   <si>
     <t>C28233</t>
+  </si>
+  <si>
+    <t>FSEL,AMP,DAC,LINE-IN,OUT2</t>
+  </si>
+  <si>
+    <t>C706875</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18">
     <font>
       <sz val="12"/>
@@ -1368,11 +1365,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I35"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1453,7 +1450,7 @@
         <v>42</v>
       </c>
       <c r="C3" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D3" t="s">
         <v>43</v>
@@ -1479,19 +1476,19 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C4" t="s">
+        <v>107</v>
+      </c>
+      <c r="D4" t="s">
         <v>108</v>
-      </c>
-      <c r="C4" t="s">
-        <v>109</v>
-      </c>
-      <c r="D4" t="s">
-        <v>110</v>
       </c>
       <c r="E4">
         <v>2</v>
       </c>
       <c r="F4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G4" t="s">
         <v>83</v>
@@ -1500,7 +1497,7 @@
         <v>12</v>
       </c>
       <c r="I4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -1598,7 +1595,7 @@
         <v>25</v>
       </c>
       <c r="C8" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D8" t="s">
         <v>9</v>
@@ -1624,28 +1621,28 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C9" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="D9" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="E9">
         <v>2</v>
       </c>
       <c r="F9" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="G9" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="H9" t="s">
         <v>12</v>
       </c>
       <c r="I9" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -1656,19 +1653,19 @@
         <v>97</v>
       </c>
       <c r="C10" t="s">
+        <v>159</v>
+      </c>
+      <c r="D10" t="s">
         <v>98</v>
       </c>
-      <c r="D10" t="s">
-        <v>99</v>
-      </c>
       <c r="E10">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H10" t="s">
         <v>12</v>
       </c>
       <c r="I10" t="s">
-        <v>100</v>
+        <v>160</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -1676,22 +1673,28 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>97</v>
+        <v>118</v>
       </c>
       <c r="C11" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
       <c r="D11" t="s">
-        <v>76</v>
+        <v>120</v>
       </c>
       <c r="E11">
         <v>1</v>
       </c>
+      <c r="F11" t="s">
+        <v>121</v>
+      </c>
+      <c r="G11" t="s">
+        <v>122</v>
+      </c>
       <c r="H11" t="s">
         <v>12</v>
       </c>
       <c r="I11" t="s">
-        <v>100</v>
+        <v>123</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -1699,28 +1702,28 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>121</v>
+        <v>67</v>
       </c>
       <c r="C12" t="s">
-        <v>122</v>
+        <v>150</v>
       </c>
       <c r="D12" t="s">
-        <v>123</v>
+        <v>140</v>
       </c>
       <c r="E12">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F12" t="s">
-        <v>124</v>
+        <v>67</v>
       </c>
       <c r="G12" t="s">
-        <v>125</v>
+        <v>68</v>
       </c>
       <c r="H12" t="s">
         <v>12</v>
       </c>
       <c r="I12" t="s">
-        <v>126</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -1728,28 +1731,28 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="C13" t="s">
-        <v>153</v>
+        <v>52</v>
       </c>
       <c r="D13" t="s">
-        <v>143</v>
+        <v>53</v>
       </c>
       <c r="E13">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F13" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="G13" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="H13" t="s">
         <v>12</v>
       </c>
       <c r="I13" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -1757,28 +1760,22 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>51</v>
+        <v>74</v>
       </c>
       <c r="C14" t="s">
-        <v>52</v>
+        <v>75</v>
       </c>
       <c r="D14" t="s">
-        <v>53</v>
+        <v>76</v>
       </c>
       <c r="E14">
-        <v>1</v>
-      </c>
-      <c r="F14" t="s">
-        <v>54</v>
-      </c>
-      <c r="G14" t="s">
-        <v>55</v>
+        <v>2</v>
       </c>
       <c r="H14" t="s">
         <v>12</v>
       </c>
       <c r="I14" t="s">
-        <v>56</v>
+        <v>77</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -1786,22 +1783,28 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>74</v>
+        <v>38</v>
       </c>
       <c r="C15" t="s">
-        <v>75</v>
+        <v>39</v>
       </c>
       <c r="D15" t="s">
-        <v>76</v>
+        <v>9</v>
       </c>
       <c r="E15">
         <v>2</v>
       </c>
+      <c r="F15" t="s">
+        <v>40</v>
+      </c>
+      <c r="G15" t="s">
+        <v>28</v>
+      </c>
       <c r="H15" t="s">
         <v>12</v>
       </c>
       <c r="I15" t="s">
-        <v>77</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -1809,28 +1812,28 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="C16" t="s">
-        <v>39</v>
+        <v>153</v>
       </c>
       <c r="D16" t="s">
-        <v>9</v>
+        <v>110</v>
       </c>
       <c r="E16">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F16" t="s">
-        <v>40</v>
+        <v>111</v>
       </c>
       <c r="G16" t="s">
-        <v>28</v>
+        <v>112</v>
       </c>
       <c r="H16" t="s">
         <v>12</v>
       </c>
       <c r="I16" t="s">
-        <v>41</v>
+        <v>113</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -1838,28 +1841,22 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>20</v>
+        <v>145</v>
       </c>
       <c r="C17" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="D17" t="s">
-        <v>113</v>
+        <v>16</v>
       </c>
       <c r="E17">
-        <v>4</v>
-      </c>
-      <c r="F17" t="s">
-        <v>114</v>
-      </c>
-      <c r="G17" t="s">
-        <v>115</v>
+        <v>2</v>
       </c>
       <c r="H17" t="s">
         <v>12</v>
       </c>
       <c r="I17" t="s">
-        <v>116</v>
+        <v>157</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -1867,22 +1864,28 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>148</v>
+        <v>114</v>
       </c>
       <c r="C18" t="s">
-        <v>149</v>
+        <v>114</v>
       </c>
       <c r="D18" t="s">
-        <v>16</v>
+        <v>115</v>
       </c>
       <c r="E18">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="F18" t="s">
+        <v>116</v>
+      </c>
+      <c r="G18" t="s">
+        <v>103</v>
       </c>
       <c r="H18" t="s">
         <v>12</v>
       </c>
       <c r="I18" t="s">
-        <v>160</v>
+        <v>117</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -1890,28 +1893,28 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="C19" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="D19" t="s">
-        <v>118</v>
+        <v>126</v>
       </c>
       <c r="E19">
         <v>1</v>
       </c>
       <c r="F19" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
       <c r="G19" t="s">
-        <v>105</v>
+        <v>128</v>
       </c>
       <c r="H19" t="s">
         <v>12</v>
       </c>
       <c r="I19" t="s">
-        <v>120</v>
+        <v>129</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -1919,28 +1922,22 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>127</v>
+        <v>70</v>
       </c>
       <c r="C20" t="s">
-        <v>128</v>
+        <v>71</v>
       </c>
       <c r="D20" t="s">
-        <v>129</v>
+        <v>72</v>
       </c>
       <c r="E20">
         <v>1</v>
       </c>
-      <c r="F20" t="s">
-        <v>130</v>
-      </c>
-      <c r="G20" t="s">
-        <v>131</v>
-      </c>
       <c r="H20" t="s">
         <v>12</v>
       </c>
       <c r="I20" t="s">
-        <v>132</v>
+        <v>73</v>
       </c>
     </row>
     <row r="21" spans="1:9">
@@ -1948,22 +1945,28 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="C21" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="D21" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="E21">
         <v>1</v>
       </c>
+      <c r="F21" t="s">
+        <v>64</v>
+      </c>
+      <c r="G21" t="s">
+        <v>65</v>
+      </c>
       <c r="H21" t="s">
         <v>12</v>
       </c>
       <c r="I21" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
     </row>
     <row r="22" spans="1:9">
@@ -1971,28 +1974,28 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>61</v>
+        <v>99</v>
       </c>
       <c r="C22" t="s">
-        <v>62</v>
+        <v>100</v>
       </c>
       <c r="D22" t="s">
-        <v>63</v>
+        <v>101</v>
       </c>
       <c r="E22">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F22" t="s">
-        <v>64</v>
+        <v>102</v>
       </c>
       <c r="G22" t="s">
-        <v>65</v>
+        <v>103</v>
       </c>
       <c r="H22" t="s">
         <v>12</v>
       </c>
       <c r="I22" t="s">
-        <v>66</v>
+        <v>104</v>
       </c>
     </row>
     <row r="23" spans="1:9">
@@ -2000,28 +2003,28 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>101</v>
+        <v>141</v>
       </c>
       <c r="C23" t="s">
-        <v>102</v>
+        <v>142</v>
       </c>
       <c r="D23" t="s">
-        <v>103</v>
+        <v>143</v>
       </c>
       <c r="E23">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F23" t="s">
-        <v>104</v>
+        <v>141</v>
       </c>
       <c r="G23" t="s">
-        <v>105</v>
+        <v>134</v>
       </c>
       <c r="H23" t="s">
         <v>12</v>
       </c>
       <c r="I23" t="s">
-        <v>106</v>
+        <v>144</v>
       </c>
     </row>
     <row r="24" spans="1:9">
@@ -2029,28 +2032,28 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>144</v>
+        <v>20</v>
       </c>
       <c r="C24" t="s">
-        <v>145</v>
+        <v>154</v>
       </c>
       <c r="D24" t="s">
-        <v>146</v>
+        <v>21</v>
       </c>
       <c r="E24">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F24" t="s">
-        <v>144</v>
+        <v>22</v>
       </c>
       <c r="G24" t="s">
-        <v>137</v>
+        <v>23</v>
       </c>
       <c r="H24" t="s">
         <v>12</v>
       </c>
       <c r="I24" t="s">
-        <v>147</v>
+        <v>24</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -2058,16 +2061,16 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>20</v>
+        <v>92</v>
       </c>
       <c r="C25" t="s">
-        <v>157</v>
+        <v>93</v>
       </c>
       <c r="D25" t="s">
         <v>21</v>
       </c>
       <c r="E25">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F25" t="s">
         <v>22</v>
@@ -2086,58 +2089,52 @@
       <c r="A26">
         <v>25</v>
       </c>
-      <c r="B26" t="s">
-        <v>92</v>
+      <c r="B26">
+        <v>100</v>
       </c>
       <c r="C26" t="s">
-        <v>93</v>
+        <v>147</v>
       </c>
       <c r="D26" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="E26">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F26" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="G26" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="H26" t="s">
         <v>12</v>
       </c>
       <c r="I26" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
     </row>
     <row r="27" spans="1:9">
       <c r="A27">
         <v>26</v>
       </c>
-      <c r="B27">
-        <v>100</v>
+      <c r="B27" t="s">
+        <v>47</v>
       </c>
       <c r="C27" t="s">
-        <v>150</v>
+        <v>48</v>
       </c>
       <c r="D27" t="s">
-        <v>16</v>
+        <v>49</v>
       </c>
       <c r="E27">
-        <v>4</v>
-      </c>
-      <c r="F27" t="s">
-        <v>30</v>
-      </c>
-      <c r="G27" t="s">
-        <v>31</v>
+        <v>1</v>
       </c>
       <c r="H27" t="s">
         <v>12</v>
       </c>
       <c r="I27" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
     </row>
     <row r="28" spans="1:9">
@@ -2145,80 +2142,86 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>47</v>
+        <v>130</v>
       </c>
       <c r="C28" t="s">
-        <v>48</v>
+        <v>131</v>
       </c>
       <c r="D28" t="s">
-        <v>49</v>
+        <v>132</v>
       </c>
       <c r="E28">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="F28" t="s">
+        <v>133</v>
+      </c>
+      <c r="G28" t="s">
+        <v>134</v>
       </c>
       <c r="H28" t="s">
         <v>12</v>
       </c>
       <c r="I28" t="s">
-        <v>50</v>
+        <v>135</v>
       </c>
     </row>
     <row r="29" spans="1:9">
       <c r="A29">
         <v>28</v>
       </c>
-      <c r="B29" t="s">
-        <v>133</v>
+      <c r="B29">
+        <v>22</v>
       </c>
       <c r="C29" t="s">
-        <v>134</v>
+        <v>86</v>
       </c>
       <c r="D29" t="s">
-        <v>135</v>
+        <v>16</v>
       </c>
       <c r="E29">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F29" t="s">
-        <v>136</v>
+        <v>87</v>
       </c>
       <c r="G29" t="s">
-        <v>137</v>
+        <v>18</v>
       </c>
       <c r="H29" t="s">
         <v>12</v>
       </c>
       <c r="I29" t="s">
-        <v>138</v>
+        <v>88</v>
       </c>
     </row>
     <row r="30" spans="1:9">
       <c r="A30">
         <v>29</v>
       </c>
-      <c r="B30">
-        <v>22</v>
+      <c r="B30" t="s">
+        <v>25</v>
       </c>
       <c r="C30" t="s">
-        <v>86</v>
+        <v>151</v>
       </c>
       <c r="D30" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="E30">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="F30" t="s">
-        <v>87</v>
+        <v>27</v>
       </c>
       <c r="G30" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="H30" t="s">
         <v>12</v>
       </c>
       <c r="I30" t="s">
-        <v>88</v>
+        <v>29</v>
       </c>
     </row>
     <row r="31" spans="1:9">
@@ -2226,28 +2229,28 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>25</v>
+        <v>57</v>
       </c>
       <c r="C31" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="D31" t="s">
         <v>26</v>
       </c>
       <c r="E31">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="F31" t="s">
-        <v>27</v>
+        <v>58</v>
       </c>
       <c r="G31" t="s">
-        <v>28</v>
+        <v>59</v>
       </c>
       <c r="H31" t="s">
         <v>12</v>
       </c>
       <c r="I31" t="s">
-        <v>29</v>
+        <v>60</v>
       </c>
     </row>
     <row r="32" spans="1:9">
@@ -2255,28 +2258,28 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>57</v>
+        <v>78</v>
       </c>
       <c r="C32" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
       <c r="D32" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="E32">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="F32" t="s">
-        <v>58</v>
+        <v>85</v>
       </c>
       <c r="G32" t="s">
-        <v>59</v>
+        <v>18</v>
       </c>
       <c r="H32" t="s">
         <v>12</v>
       </c>
       <c r="I32" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
     </row>
     <row r="33" spans="1:9">
@@ -2284,28 +2287,22 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>78</v>
+        <v>25</v>
       </c>
       <c r="C33" t="s">
-        <v>151</v>
+        <v>105</v>
       </c>
       <c r="D33" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E33">
-        <v>11</v>
-      </c>
-      <c r="F33" t="s">
-        <v>85</v>
-      </c>
-      <c r="G33" t="s">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="H33" t="s">
         <v>12</v>
       </c>
       <c r="I33" t="s">
-        <v>79</v>
+        <v>158</v>
       </c>
     </row>
     <row r="34" spans="1:9">
@@ -2313,55 +2310,32 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="C34" t="s">
-        <v>107</v>
+        <v>34</v>
       </c>
       <c r="D34" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="E34">
         <v>1</v>
       </c>
+      <c r="F34" t="s">
+        <v>35</v>
+      </c>
+      <c r="G34" t="s">
+        <v>36</v>
+      </c>
       <c r="H34" t="s">
         <v>12</v>
       </c>
       <c r="I34" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9">
-      <c r="A35">
-        <v>34</v>
-      </c>
-      <c r="B35" t="s">
-        <v>33</v>
-      </c>
-      <c r="C35" t="s">
-        <v>34</v>
-      </c>
-      <c r="D35" t="s">
-        <v>16</v>
-      </c>
-      <c r="E35">
-        <v>1</v>
-      </c>
-      <c r="F35" t="s">
-        <v>35</v>
-      </c>
-      <c r="G35" t="s">
-        <v>36</v>
-      </c>
-      <c r="H35" t="s">
-        <v>12</v>
-      </c>
-      <c r="I35" t="s">
         <v>37</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I37"/>
+  <autoFilter ref="A1:I36" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>